<commit_message>
Updated examples to include error count
</commit_message>
<xml_diff>
--- a/examples/gun offenders/counters.xlsx
+++ b/examples/gun offenders/counters.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,7 +757,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Error: Value '2/18/2011' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
+          <t>Error: Value '02/18/2011' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Error: Value '7/26/2010' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
+          <t>Error: Value '07/26/2010' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Error: Value '4/13/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
+          <t>Error: Value '04/13/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Error: Value '3/28/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
+          <t>Error: Value '03/28/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Error: Value '7/18/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
+          <t>Error: Value '07/18/2012' does not match regex '^(((0?[1-9]|[12]\d|3[01])[\.\-\/](0?[13578]|1[02])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|[12]\d|30)[\.\-\/](0?[13456789]|1[012])[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|((0?[1-9]|1\d|2[0-8])[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?\d{2}|\d))|(29[\.\-\/]0?2[\.\-\/]((1[6-9]|[2-9]\d)?(0[48]|[2468][048]|[13579][26])|((16|[2468][048]|[3579][26])00)|00|[048])))$'</t>
         </is>
       </c>
     </row>
@@ -1551,12 +1551,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Completeness of Mandatory fields</t>
+          <t>Meta Compliance (data type)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+          <t>Error: Value '' is not an int. An int was expected</t>
         </is>
       </c>
     </row>
@@ -1585,19 +1585,19 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Completeness of Mandatory fields</t>
+          <t>Meta Compliance (data type)</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+          <t>Error: Value '' is not an int. An int was expected</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>neighborhood</t>
+          <t>post</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1614,24 +1614,24 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>neighborhood</t>
+          <t>post</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Completeness of Mandatory fields</t>
+          <t>Meta Compliance (data type)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+          <t>Error: Value '' is not an int. An int was expected</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>neighborhood</t>
+          <t>post</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1648,24 +1648,24 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>neighborhood</t>
+          <t>post</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Completeness of Mandatory fields</t>
+          <t>Meta Compliance (data type)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+          <t>Error: Value '' is not an int. An int was expected</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Location 1</t>
+          <t>neighborhood</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1682,7 +1682,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Location 1</t>
+          <t>neighborhood</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1699,7 +1699,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Location 1</t>
+          <t>neighborhood</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1716,15 +1716,83 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>neighborhood</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Completeness of Mandatory fields</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
           <t>Location 1</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Completeness of Mandatory fields</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Completeness of Mandatory fields</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Location 1</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Completeness of Mandatory fields</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Location 1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Completeness of Mandatory fields</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Location 1</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Completeness of Mandatory fields</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
         <is>
           <t>Error: Mandatory field is BLANK or NULL. A value is required.</t>
         </is>

</xml_diff>